<commit_message>
Script v2 using only mouse and keyboard
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>YES</t>
   </si>
@@ -62,6 +62,9 @@
 Noticing this was a February 15th inception date for this opportunity, could you let us know whether we have received a submission for this lead, and if yes, we have quoted?_x000D_
 _x000D_
 FYI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="AA1:AH10"/>
+  <dimension ref="X1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,7 +897,7 @@
     <col min="34" max="34" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="27:34" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="24:34" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AA1" t="s">
         <v>7</v>
       </c>
@@ -908,7 +911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="27:34" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="24:34" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AA2" t="s">
         <v>7</v>
       </c>
@@ -922,7 +925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="27:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="24:34" x14ac:dyDescent="0.3">
       <c r="AA3" t="s">
         <v>7</v>
       </c>
@@ -936,7 +939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="27:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="24:34" x14ac:dyDescent="0.3">
       <c r="AA4" t="s">
         <v>7</v>
       </c>
@@ -950,7 +953,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="27:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="24:34" x14ac:dyDescent="0.3">
+      <c r="X5" t="s">
+        <v>14</v>
+      </c>
       <c r="AA5" t="s">
         <v>7</v>
       </c>
@@ -964,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="27:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="24:34" x14ac:dyDescent="0.3">
       <c r="AA6" t="s">
         <v>7</v>
       </c>
@@ -972,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="27:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="24:34" x14ac:dyDescent="0.3">
       <c r="AA7" t="s">
         <v>7</v>
       </c>
@@ -980,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="27:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="24:34" x14ac:dyDescent="0.35">
       <c r="AA8" t="s">
         <v>7</v>
       </c>
@@ -988,7 +994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="27:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="24:34" x14ac:dyDescent="0.3">
       <c r="AA9" t="s">
         <v>7</v>
       </c>
@@ -996,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="27:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="24:34" x14ac:dyDescent="0.35">
       <c r="AA10" t="s">
         <v>7</v>
       </c>
@@ -1011,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,51 +1037,6 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>